<commit_message>
nuttcp simplification and results
</commit_message>
<xml_diff>
--- a/nuttcp/results/nuttcp.xlsx
+++ b/nuttcp/results/nuttcp.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
   <si>
     <t>C-&gt;S</t>
   </si>
@@ -42,13 +42,7 @@
     <t>S-&gt;C</t>
   </si>
   <si>
-    <t>KVM vhost</t>
-  </si>
-  <si>
     <t>Connections</t>
-  </si>
-  <si>
-    <t>Fuck! The wrong row is hidden and I can't unhide it!</t>
   </si>
 </sst>
 </file>
@@ -204,10 +198,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>9356.65</c:v>
+                  <c:v>9.3481319</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.328518200000001</c:v>
+                  <c:v>9.340229600000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -249,7 +243,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>7120.1038</c:v>
+                  <c:v>9.3298451</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.0</c:v>
@@ -302,7 +296,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>KVM vhost</c:v>
+                  <c:v>KVM</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -328,8 +322,11 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>9.2942403</c:v>
+                </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>9.264935400000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -344,11 +341,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2135486952"/>
-        <c:axId val="-2135485352"/>
+        <c:axId val="2091038984"/>
+        <c:axId val="2091035848"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2135486952"/>
+        <c:axId val="2091038984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -357,7 +354,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2135485352"/>
+        <c:crossAx val="2091035848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -365,7 +362,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2135485352"/>
+        <c:axId val="2091035848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -376,7 +373,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2135486952"/>
+        <c:crossAx val="2091038984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -570,11 +567,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2140455848"/>
-        <c:axId val="2072275976"/>
+        <c:axId val="2090988360"/>
+        <c:axId val="2090985368"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2140455848"/>
+        <c:axId val="2090988360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -584,12 +581,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2072275976"/>
+        <c:crossAx val="2090985368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2072275976"/>
+        <c:axId val="2090985368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -600,7 +597,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2140455848"/>
+        <c:crossAx val="2090988360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1018,10 +1015,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:N24"/>
+  <dimension ref="A4:N24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1029,11 +1026,6 @@
     <col min="4" max="4" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-    </row>
     <row r="4" spans="1:14">
       <c r="A4" t="s">
         <v>1</v>
@@ -1048,7 +1040,7 @@
         <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="L4" t="s">
         <v>2</v>
@@ -1060,31 +1052,34 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" hidden="1">
       <c r="A5" t="s">
         <v>0</v>
       </c>
       <c r="B5">
-        <v>9356.65</v>
+        <v>9348.1319000000003</v>
       </c>
       <c r="C5">
-        <v>7120.1037999999999</v>
+        <v>9329.8451000000005</v>
+      </c>
+      <c r="E5">
+        <v>9294.2402999999995</v>
       </c>
       <c r="K5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14" hidden="1">
+    <row r="6" spans="1:14">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B6">
         <f>B5/1000</f>
-        <v>9.3566500000000001</v>
+        <v>9.3481319000000003</v>
       </c>
       <c r="C6">
         <f>C5/1000</f>
-        <v>7.1201037999999999</v>
+        <v>9.3298451</v>
       </c>
       <c r="D6">
         <f>D5/1000</f>
@@ -1092,7 +1087,7 @@
       </c>
       <c r="E6">
         <f>E5/1000</f>
-        <v>0</v>
+        <v>9.2942403000000002</v>
       </c>
     </row>
     <row r="7" spans="1:14" hidden="1">
@@ -1100,7 +1095,10 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>9328.5182000000004</v>
+        <v>9340.2296000000006</v>
+      </c>
+      <c r="E7">
+        <v>9264.9354000000003</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -1109,7 +1107,7 @@
       </c>
       <c r="B8">
         <f>B7/1000</f>
-        <v>9.3285182000000013</v>
+        <v>9.3402296000000007</v>
       </c>
       <c r="C8">
         <f>C7/1000</f>
@@ -1121,7 +1119,7 @@
       </c>
       <c r="E8">
         <f>E7/1000</f>
-        <v>0</v>
+        <v>9.2649354000000006</v>
       </c>
       <c r="K8">
         <v>2</v>
@@ -1156,7 +1154,7 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B19" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
nuttcp: got docker server->client working, added the missing bar
</commit_message>
<xml_diff>
--- a/nuttcp/results/nuttcp.xlsx
+++ b/nuttcp/results/nuttcp.xlsx
@@ -246,7 +246,7 @@
                   <c:v>9.3298451</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>9.3199298</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -341,11 +341,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2091038984"/>
-        <c:axId val="2091035848"/>
+        <c:axId val="2067579576"/>
+        <c:axId val="2067582744"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2091038984"/>
+        <c:axId val="2067579576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -354,7 +354,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2091035848"/>
+        <c:crossAx val="2067582744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -362,9 +362,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2091035848"/>
+        <c:axId val="2067582744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -373,9 +374,10 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2091038984"/>
+        <c:crossAx val="2067579576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:minorUnit val="0.2"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -567,11 +569,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2090988360"/>
-        <c:axId val="2090985368"/>
+        <c:axId val="2067646824"/>
+        <c:axId val="2067649816"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2090988360"/>
+        <c:axId val="2067646824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -581,12 +583,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2090985368"/>
+        <c:crossAx val="2067649816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2090985368"/>
+        <c:axId val="2067649816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -597,7 +599,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2090988360"/>
+        <c:crossAx val="2067646824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1018,7 +1020,7 @@
   <dimension ref="A4:N24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1097,6 +1099,9 @@
       <c r="B7">
         <v>9340.2296000000006</v>
       </c>
+      <c r="C7">
+        <v>9319.9297999999999</v>
+      </c>
       <c r="E7">
         <v>9264.9354000000003</v>
       </c>
@@ -1111,7 +1116,7 @@
       </c>
       <c r="C8">
         <f>C7/1000</f>
-        <v>0</v>
+        <v>9.3199298000000006</v>
       </c>
       <c r="D8">
         <f>D7/1000</f>

</xml_diff>